<commit_message>
Enemy data research and updated bubble bobble map fixer to also export enemy data in a seperated file
</commit_message>
<xml_diff>
--- a/BubbleBobbleResearch/CharactersToSpawnPerLevel.xlsx
+++ b/BubbleBobbleResearch/CharactersToSpawnPerLevel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NickyFieu\Desktop\dae\2ndYear\Prog4\Code Pain\BubbleBobbleResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63863BA7-9EC4-44FF-BBCE-261406ED681D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1367590D-84F9-462E-9B78-8DBCC407E6EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5CA7CAEA-36DB-4171-9CFF-42A84394C5FE}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="183">
   <si>
     <t>L1</t>
   </si>
@@ -425,147 +425,30 @@
     <t>4 MI</t>
   </si>
   <si>
-    <t>3 ZC 3 MO</t>
-  </si>
-  <si>
-    <t>3 ZC 4 MO</t>
-  </si>
-  <si>
     <t>6 MO</t>
   </si>
   <si>
-    <t>7 MO</t>
-  </si>
-  <si>
-    <t>5 MO 2 MI</t>
-  </si>
-  <si>
-    <t>5 ZC 2 MI</t>
-  </si>
-  <si>
     <t>3 P 2 MI</t>
   </si>
   <si>
-    <t>4 ZC 3 MI</t>
-  </si>
-  <si>
-    <t>7 MI</t>
-  </si>
-  <si>
     <t>4P</t>
   </si>
   <si>
     <t>5P</t>
   </si>
   <si>
-    <t>7P</t>
-  </si>
-  <si>
-    <t>4 MO 3 P</t>
-  </si>
-  <si>
-    <t>6 MO 1 MI</t>
-  </si>
-  <si>
-    <t>5 BA 2 P</t>
-  </si>
-  <si>
-    <t>7 ZC</t>
-  </si>
-  <si>
-    <t>7 BA</t>
-  </si>
-  <si>
-    <t>5 HI 2 MI</t>
-  </si>
-  <si>
     <t>6P</t>
   </si>
   <si>
-    <t>7 D</t>
-  </si>
-  <si>
-    <t>7 HI</t>
-  </si>
-  <si>
-    <t>2 MO 2 MI 2 HI 1 BA</t>
-  </si>
-  <si>
     <t>4 HI 2 MI</t>
   </si>
   <si>
-    <t>3 HI 4 BA</t>
-  </si>
-  <si>
-    <t>5 D 2 HI</t>
-  </si>
-  <si>
-    <t>3 MI 4 ZC</t>
-  </si>
-  <si>
-    <t>1 ZC 1 MI 2 MO 1 P 1 BA 1HI</t>
-  </si>
-  <si>
-    <t>2 ZC 1 HI 2 P 1 MI 1 MO</t>
-  </si>
-  <si>
     <t>4 IN</t>
   </si>
   <si>
-    <t>7 IN</t>
-  </si>
-  <si>
-    <t>3 IN 4 D</t>
-  </si>
-  <si>
-    <t>5 IN</t>
-  </si>
-  <si>
-    <t>2 IN 3 D 2 HI</t>
-  </si>
-  <si>
-    <t>3 HI 4 P</t>
-  </si>
-  <si>
-    <t>4 HI 2D 1 IN</t>
-  </si>
-  <si>
-    <t>3 IN 2 MI 2 BA</t>
-  </si>
-  <si>
-    <t>4 BA 3 MI</t>
-  </si>
-  <si>
-    <t>2 ZC 3 BA 2 P</t>
-  </si>
-  <si>
-    <t>3 HI 2 BA 2 P</t>
-  </si>
-  <si>
-    <t>5 IN 1 MI 1 BA</t>
-  </si>
-  <si>
-    <t>2 IN 2 MO 3 P</t>
-  </si>
-  <si>
-    <t>1 IN 6 D</t>
-  </si>
-  <si>
-    <t>Numbers of Enemies per level ( NO SPECIAL LEVELS )</t>
-  </si>
-  <si>
     <t>6 HI</t>
   </si>
   <si>
-    <t>4 D 3 IN</t>
-  </si>
-  <si>
-    <t>2 IN 2 D 1 MO 2 ZC</t>
-  </si>
-  <si>
-    <t>4 MO 2 D 1 P</t>
-  </si>
-  <si>
     <t>1 SD</t>
   </si>
   <si>
@@ -588,6 +471,117 @@
   </si>
   <si>
     <t>3 ZC ?</t>
+  </si>
+  <si>
+    <t>5 MI</t>
+  </si>
+  <si>
+    <t>4 ZC 2 MO</t>
+  </si>
+  <si>
+    <t>2 ZC 4 MO</t>
+  </si>
+  <si>
+    <t>4 MO 2 MI</t>
+  </si>
+  <si>
+    <t>Numbers of Enemies per level AMIGA VERSION! ( NO SPECIAL LEVELS )</t>
+  </si>
+  <si>
+    <t>4 ZC 2 MI</t>
+  </si>
+  <si>
+    <t>6 MI</t>
+  </si>
+  <si>
+    <t>4 MO 2 P</t>
+  </si>
+  <si>
+    <t>5 MO 1 MI</t>
+  </si>
+  <si>
+    <t>5 BA 1 P</t>
+  </si>
+  <si>
+    <t>6 BA</t>
+  </si>
+  <si>
+    <t>2 MO 2 MI 2 HI</t>
+  </si>
+  <si>
+    <t>4 HI 2 BA</t>
+  </si>
+  <si>
+    <t>6 D</t>
+  </si>
+  <si>
+    <t>2 MI 4 ZC</t>
+  </si>
+  <si>
+    <t>4 D 2 HI</t>
+  </si>
+  <si>
+    <t>1 MI 2 MO 1 P 1 BA 1HI</t>
+  </si>
+  <si>
+    <t>3 MI 3 ZC</t>
+  </si>
+  <si>
+    <t>2 ZC 1 HI 2 P 1 MI</t>
+  </si>
+  <si>
+    <t>6 IN</t>
+  </si>
+  <si>
+    <t>2 IN 4 D</t>
+  </si>
+  <si>
+    <t>2 IN 2 D 2 HI</t>
+  </si>
+  <si>
+    <t>2 HI 4 P</t>
+  </si>
+  <si>
+    <t>2 IN 2 MI 2 BA</t>
+  </si>
+  <si>
+    <t>4 HI 2D</t>
+  </si>
+  <si>
+    <t>4 BA 2 MI</t>
+  </si>
+  <si>
+    <t>4 BA 2 P</t>
+  </si>
+  <si>
+    <t>2 HI 2 BA 2 P</t>
+  </si>
+  <si>
+    <t>2 ZC 3 BA 1 P</t>
+  </si>
+  <si>
+    <t>4 IN 1 MI 1 BA</t>
+  </si>
+  <si>
+    <t>2 IN 2 MO 2 P</t>
+  </si>
+  <si>
+    <t>1 IN 5 D</t>
+  </si>
+  <si>
+    <t>2 D 2 IN 2 ZC</t>
+  </si>
+  <si>
+    <t>2 IN 1 D 1 MO 2 ZC</t>
+  </si>
+  <si>
+    <t>3 MO 2 D 1 P</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Drops?</t>
   </si>
 </sst>
 </file>
@@ -794,6 +788,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -821,18 +824,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1147,10 +1141,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67BD1ADB-60D6-4770-8E3D-50D34901488F}">
-  <dimension ref="B2:U29"/>
+  <dimension ref="B2:U38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31:M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1158,8 +1152,8 @@
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="17.7109375" bestFit="1" customWidth="1"/>
@@ -1176,813 +1170,980 @@
         <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>131</v>
+        <v>148</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>30</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="K2" s="17" t="s">
-        <v>141</v>
+      <c r="K2" s="7" t="s">
+        <v>134</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M2" s="16" t="s">
-        <v>149</v>
+      <c r="M2" s="6" t="s">
+        <v>159</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="O2" s="16" t="s">
-        <v>159</v>
+      <c r="O2" s="6" t="s">
+        <v>165</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="Q2" s="16" t="s">
-        <v>167</v>
+      <c r="Q2" s="6" t="s">
+        <v>174</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="S2" s="16" t="s">
-        <v>150</v>
+      <c r="S2" s="6" t="s">
+        <v>137</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>90</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="4" t="s">
         <v>101</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="13" t="s">
-        <v>132</v>
+      <c r="E3" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="13" t="s">
-        <v>139</v>
+      <c r="G3" s="4" t="s">
+        <v>132</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="13" t="s">
-        <v>141</v>
+      <c r="I3" s="4" t="s">
+        <v>134</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K3" s="18" t="s">
-        <v>150</v>
+      <c r="K3" s="8" t="s">
+        <v>137</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="M3" s="18" t="s">
-        <v>149</v>
+      <c r="M3" s="8" t="s">
+        <v>159</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="O3" s="18" t="s">
-        <v>160</v>
+      <c r="O3" s="8" t="s">
+        <v>166</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="Q3" s="18" t="s">
-        <v>144</v>
+      <c r="Q3" s="8" t="s">
+        <v>172</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="S3" s="18" t="s">
-        <v>171</v>
+      <c r="S3" s="8" t="s">
+        <v>166</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="U3" s="13" t="s">
-        <v>145</v>
+      <c r="U3" s="4" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="4" t="s">
         <v>101</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="13" t="s">
-        <v>133</v>
+      <c r="E4" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="13" t="s">
-        <v>140</v>
+      <c r="G4" s="4" t="s">
+        <v>133</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I4" s="13" t="s">
-        <v>145</v>
+      <c r="I4" s="4" t="s">
+        <v>102</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K4" s="18" t="s">
-        <v>151</v>
+      <c r="K4" s="8" t="s">
+        <v>157</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="M4" s="18" t="s">
-        <v>141</v>
+      <c r="M4" s="8" t="s">
+        <v>134</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="O4" s="18" t="s">
-        <v>159</v>
+      <c r="O4" s="8" t="s">
+        <v>165</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="Q4" s="18" t="s">
-        <v>168</v>
+      <c r="Q4" s="8" t="s">
+        <v>173</v>
       </c>
       <c r="R4" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="S4" s="18" t="s">
-        <v>171</v>
+      <c r="S4" s="8" t="s">
+        <v>177</v>
       </c>
       <c r="T4" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="U4" s="13" t="s">
-        <v>141</v>
+      <c r="U4" s="4" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="4" t="s">
         <v>102</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>134</v>
+      <c r="E5" s="4" t="s">
+        <v>149</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="13" t="s">
-        <v>141</v>
+      <c r="G5" s="4" t="s">
+        <v>134</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I5" s="13" t="s">
-        <v>138</v>
+      <c r="I5" s="4" t="s">
+        <v>152</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K5" s="18" t="s">
-        <v>150</v>
+      <c r="K5" s="8" t="s">
+        <v>137</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="M5" s="19" t="s">
-        <v>154</v>
+      <c r="M5" s="9" t="s">
+        <v>161</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="O5" s="18" t="s">
-        <v>161</v>
+      <c r="O5" s="8" t="s">
+        <v>165</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="Q5" s="18" t="s">
-        <v>138</v>
+      <c r="Q5" s="8" t="s">
+        <v>152</v>
       </c>
       <c r="R5" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="S5" s="18" t="s">
-        <v>159</v>
+      <c r="S5" s="8" t="s">
+        <v>165</v>
       </c>
       <c r="T5" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="U5" s="13" t="s">
-        <v>145</v>
+      <c r="U5" s="4" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="4" t="s">
         <v>101</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>135</v>
+      <c r="E6" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="13" t="s">
-        <v>132</v>
+      <c r="G6" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="13" t="s">
-        <v>145</v>
+      <c r="I6" s="4" t="s">
+        <v>102</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K6" s="18" t="s">
-        <v>145</v>
+      <c r="K6" s="8" t="s">
+        <v>102</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="M6" s="19" t="s">
-        <v>155</v>
+      <c r="M6" s="9" t="s">
+        <v>160</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="O6" s="18" t="s">
-        <v>162</v>
+      <c r="O6" s="8" t="s">
+        <v>167</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="Q6" s="18" t="s">
-        <v>149</v>
+      <c r="Q6" s="8" t="s">
+        <v>159</v>
       </c>
       <c r="R6" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="S6" s="18" t="s">
-        <v>159</v>
+      <c r="S6" s="8" t="s">
+        <v>165</v>
       </c>
       <c r="T6" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="U6" s="13" t="s">
-        <v>174</v>
+      <c r="U6" s="4" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="4" t="s">
         <v>103</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="13" t="s">
-        <v>133</v>
+      <c r="E7" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="13" t="s">
-        <v>138</v>
+      <c r="G7" s="4" t="s">
+        <v>152</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I7" s="13" t="s">
-        <v>146</v>
+      <c r="I7" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K7" s="18" t="s">
-        <v>146</v>
+      <c r="K7" s="8" t="s">
+        <v>156</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="M7" s="19" t="s">
-        <v>156</v>
+      <c r="M7" s="9" t="s">
+        <v>162</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="O7" s="18" t="s">
-        <v>163</v>
+      <c r="O7" s="8" t="s">
+        <v>168</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="Q7" s="18" t="s">
-        <v>169</v>
+      <c r="Q7" s="8" t="s">
+        <v>175</v>
       </c>
       <c r="R7" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="S7" s="18" t="s">
-        <v>133</v>
+      <c r="S7" s="8" t="s">
+        <v>130</v>
       </c>
       <c r="T7" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="U7" s="13" t="s">
-        <v>159</v>
+      <c r="U7" s="4" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="4" t="s">
         <v>129</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="13" t="s">
-        <v>134</v>
+      <c r="E8" s="4" t="s">
+        <v>149</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="13" t="s">
-        <v>142</v>
+      <c r="G8" s="4" t="s">
+        <v>153</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I8" s="13" t="s">
-        <v>145</v>
+      <c r="I8" s="4" t="s">
+        <v>102</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K8" s="18" t="s">
-        <v>153</v>
+      <c r="K8" s="8" t="s">
+        <v>158</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="M8" s="19" t="s">
-        <v>137</v>
+      <c r="M8" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="O8" s="18" t="s">
-        <v>165</v>
+      <c r="O8" s="8" t="s">
+        <v>169</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="Q8" s="18" t="s">
-        <v>170</v>
+      <c r="Q8" s="8" t="s">
+        <v>176</v>
       </c>
       <c r="R8" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="S8" s="20" t="s">
-        <v>141</v>
+      <c r="S8" s="10" t="s">
+        <v>134</v>
       </c>
       <c r="T8" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="U8" s="13" t="s">
-        <v>175</v>
+      <c r="U8" s="4" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="4" t="s">
         <v>103</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="4" t="s">
         <v>102</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="13" t="s">
-        <v>138</v>
+      <c r="G9" s="4" t="s">
+        <v>152</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I9" s="13" t="s">
-        <v>146</v>
+      <c r="I9" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K9" s="18" t="s">
-        <v>152</v>
+      <c r="K9" s="8" t="s">
+        <v>135</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="M9" s="19" t="s">
-        <v>149</v>
+      <c r="M9" s="9" t="s">
+        <v>163</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="O9" s="18" t="s">
-        <v>164</v>
+      <c r="O9" s="8" t="s">
+        <v>170</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="Q9" s="18" t="s">
-        <v>159</v>
+      <c r="Q9" s="8" t="s">
+        <v>165</v>
       </c>
       <c r="R9" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="S9" s="18" t="s">
-        <v>145</v>
+      <c r="S9" s="8" t="s">
+        <v>102</v>
       </c>
       <c r="T9" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="U9" s="13" t="s">
-        <v>149</v>
+      <c r="U9" s="4" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="13" t="s">
-        <v>102</v>
+      <c r="C10" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="13" t="s">
-        <v>133</v>
+      <c r="E10" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="13" t="s">
-        <v>143</v>
+      <c r="G10" s="4" t="s">
+        <v>154</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I10" s="13" t="s">
-        <v>145</v>
+      <c r="I10" s="4" t="s">
+        <v>102</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="K10" s="18" t="s">
-        <v>148</v>
+      <c r="K10" s="8" t="s">
+        <v>134</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="M10" s="19" t="s">
-        <v>157</v>
+      <c r="M10" s="9" t="s">
+        <v>164</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="O10" s="18" t="s">
-        <v>166</v>
+      <c r="O10" s="8" t="s">
+        <v>171</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="Q10" s="18" t="s">
-        <v>133</v>
+      <c r="Q10" s="8" t="s">
+        <v>130</v>
       </c>
       <c r="R10" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="S10" s="18" t="s">
-        <v>150</v>
+      <c r="S10" s="8" t="s">
+        <v>137</v>
       </c>
       <c r="T10" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="U10" s="13" t="s">
-        <v>176</v>
+      <c r="U10" s="4" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>130</v>
+      <c r="C11" s="4" t="s">
+        <v>147</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="13" t="s">
-        <v>136</v>
+      <c r="E11" s="4" t="s">
+        <v>131</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="13" t="s">
-        <v>144</v>
+      <c r="G11" s="4" t="s">
+        <v>155</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I11" s="13" t="s">
-        <v>147</v>
+      <c r="I11" s="4" t="s">
+        <v>135</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="K11" s="18" t="s">
-        <v>149</v>
+      <c r="K11" s="8" t="s">
+        <v>159</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="M11" s="19" t="s">
-        <v>158</v>
+      <c r="M11" s="9" t="s">
+        <v>136</v>
       </c>
       <c r="N11" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="O11" s="18" t="s">
-        <v>146</v>
+      <c r="O11" s="8" t="s">
+        <v>156</v>
       </c>
       <c r="P11" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="Q11" s="18" t="s">
-        <v>145</v>
+      <c r="Q11" s="8" t="s">
+        <v>102</v>
       </c>
       <c r="R11" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="S11" s="18" t="s">
-        <v>173</v>
+      <c r="S11" s="8" t="s">
+        <v>137</v>
       </c>
       <c r="T11" s="2" t="s">
         <v>99</v>
       </c>
       <c r="U11" s="3" t="s">
-        <v>177</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="5"/>
-      <c r="U12" s="6"/>
+      <c r="B12" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14"/>
+      <c r="U12" s="15"/>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="6"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="15"/>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="F14" s="4" t="s">
+      <c r="D14" s="17"/>
+      <c r="F14" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="G14" s="6"/>
+      <c r="G14" s="15"/>
       <c r="H14" s="1" t="s">
-        <v>184</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="O15" s="15"/>
+      <c r="D15" s="19"/>
+      <c r="O15" s="5"/>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="D16" s="10"/>
+      <c r="D16" s="19"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="D17" s="10"/>
+      <c r="D17" s="19"/>
+      <c r="J17" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="D18" s="10"/>
+      <c r="D18" s="19"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="D19" s="10"/>
+      <c r="D19" s="19"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="D20" s="10"/>
+      <c r="D20" s="19"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="D21" s="12"/>
+      <c r="D21" s="21"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="6"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="15"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="22"/>
+      <c r="M23" s="22"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="14" t="s">
-        <v>179</v>
-      </c>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="22"/>
+      <c r="M24" s="22"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="D25" s="12"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="22"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="21" t="s">
+      <c r="B28" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="11" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B29" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B29" s="14" t="s">
-        <v>181</v>
-      </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="22" t="s">
-        <v>183</v>
-      </c>
+      <c r="C31" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="D31" s="17"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
+      <c r="L31" s="22"/>
+      <c r="M31" s="22"/>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="D32" s="19"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="22"/>
+      <c r="L32" s="22"/>
+      <c r="M32" s="22"/>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="D33" s="19"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="22"/>
+      <c r="L33" s="22"/>
+      <c r="M33" s="22"/>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D34" s="19"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="22"/>
+      <c r="L34" s="22"/>
+      <c r="M34" s="22"/>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D35" s="19"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
+      <c r="L35" s="22"/>
+      <c r="M35" s="22"/>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="D36" s="19"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="22"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="22"/>
+      <c r="L36" s="22"/>
+      <c r="M36" s="22"/>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="D37" s="19"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="22"/>
+      <c r="J37" s="22"/>
+      <c r="K37" s="22"/>
+      <c r="L37" s="22"/>
+      <c r="M37" s="22"/>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="D38" s="21"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="22"/>
+      <c r="J38" s="22"/>
+      <c r="K38" s="22"/>
+      <c r="L38" s="22"/>
+      <c r="M38" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="36">
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="E31:M31"/>
+    <mergeCell ref="E32:M32"/>
+    <mergeCell ref="E33:M33"/>
+    <mergeCell ref="E34:M34"/>
+    <mergeCell ref="E35:M35"/>
+    <mergeCell ref="E36:M36"/>
+    <mergeCell ref="E38:M38"/>
+    <mergeCell ref="E37:M37"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="C31:D31"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
@@ -1999,10 +2160,6 @@
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
More research into bubble bobble level data / cleaning code / making code consistent
</commit_message>
<xml_diff>
--- a/BubbleBobbleResearch/CharactersToSpawnPerLevel.xlsx
+++ b/BubbleBobbleResearch/CharactersToSpawnPerLevel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NickyFieu\Desktop\dae\2ndYear\Prog4\Code Pain\BubbleBobbleResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1367590D-84F9-462E-9B78-8DBCC407E6EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3877973-D45D-45F8-B40F-351478C4E904}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5CA7CAEA-36DB-4171-9CFF-42A84394C5FE}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11385" xr2:uid="{5CA7CAEA-36DB-4171-9CFF-42A84394C5FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="186">
   <si>
     <t>L1</t>
   </si>
@@ -582,6 +582,15 @@
   </si>
   <si>
     <t>Drops?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Required to drop watermelon </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Required to drop french fries </t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -797,21 +806,6 @@
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -825,6 +819,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1143,8 +1152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67BD1ADB-60D6-4770-8E3D-50D34901488F}">
   <dimension ref="B2:U38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31:M31"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1780,48 +1789,48 @@
       </c>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="14"/>
-      <c r="S12" s="14"/>
-      <c r="T12" s="14"/>
-      <c r="U12" s="15"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="21"/>
+      <c r="S12" s="21"/>
+      <c r="T12" s="21"/>
+      <c r="U12" s="22"/>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="15"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="22"/>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="D14" s="17"/>
-      <c r="F14" s="13" t="s">
+      <c r="D14" s="19"/>
+      <c r="F14" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="G14" s="15"/>
+      <c r="G14" s="22"/>
       <c r="H14" s="1" t="s">
         <v>145</v>
       </c>
@@ -1830,29 +1839,29 @@
       <c r="B15" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="D15" s="19"/>
+      <c r="D15" s="14"/>
       <c r="O15" s="5"/>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="D16" s="19"/>
+      <c r="D16" s="14"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="D17" s="19"/>
+      <c r="D17" s="14"/>
       <c r="J17" t="s">
         <v>181</v>
       </c>
@@ -1861,119 +1870,119 @@
       <c r="B18" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="D18" s="19"/>
+      <c r="D18" s="14"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="D19" s="19"/>
+      <c r="D19" s="14"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="D20" s="19"/>
+      <c r="D20" s="14"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="D21" s="21"/>
+      <c r="D21" s="16"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="15"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="22"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="D23" s="17"/>
-      <c r="E23" s="22" t="s">
+      <c r="D23" s="19"/>
+      <c r="E23" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="22"/>
-      <c r="L23" s="22"/>
-      <c r="M23" s="22"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="D24" s="19"/>
-      <c r="E24" s="22" t="s">
+      <c r="D24" s="14"/>
+      <c r="E24" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="22"/>
-      <c r="L24" s="22"/>
-      <c r="M24" s="22"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="D25" s="21"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
-      <c r="K25" s="22"/>
-      <c r="L25" s="22"/>
-      <c r="M25" s="22"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="17"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
       <c r="E28" s="11" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
       <c r="E29" s="12" t="s">
         <v>144</v>
       </c>
@@ -1982,148 +1991,185 @@
       <c r="B31" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="C31" s="16" t="s">
+      <c r="C31" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="D31" s="17"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="22"/>
-      <c r="J31" s="22"/>
-      <c r="K31" s="22"/>
-      <c r="L31" s="22"/>
-      <c r="M31" s="22"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17"/>
+      <c r="L31" s="17"/>
+      <c r="M31" s="17"/>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="D32" s="19"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="22"/>
-      <c r="J32" s="22"/>
-      <c r="K32" s="22"/>
-      <c r="L32" s="22"/>
-      <c r="M32" s="22"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="17"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="17"/>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C33" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="D33" s="19"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="22"/>
-      <c r="I33" s="22"/>
-      <c r="J33" s="22"/>
-      <c r="K33" s="22"/>
-      <c r="L33" s="22"/>
-      <c r="M33" s="22"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="17"/>
+      <c r="L33" s="17"/>
+      <c r="M33" s="17"/>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C34" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="D34" s="19"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="22"/>
-      <c r="I34" s="22"/>
-      <c r="J34" s="22"/>
-      <c r="K34" s="22"/>
-      <c r="L34" s="22"/>
-      <c r="M34" s="22"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="17"/>
+      <c r="L34" s="17"/>
+      <c r="M34" s="17"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="C35" s="18" t="s">
+      <c r="C35" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="D35" s="19"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="22"/>
-      <c r="I35" s="22"/>
-      <c r="J35" s="22"/>
-      <c r="K35" s="22"/>
-      <c r="L35" s="22"/>
-      <c r="M35" s="22"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
+      <c r="K35" s="17"/>
+      <c r="L35" s="17"/>
+      <c r="M35" s="17"/>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="C36" s="18" t="s">
+      <c r="C36" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="D36" s="19"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="22"/>
-      <c r="I36" s="22"/>
-      <c r="J36" s="22"/>
-      <c r="K36" s="22"/>
-      <c r="L36" s="22"/>
-      <c r="M36" s="22"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="17"/>
+      <c r="L36" s="17"/>
+      <c r="M36" s="17"/>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="C37" s="18" t="s">
+      <c r="C37" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="D37" s="19"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="22"/>
-      <c r="J37" s="22"/>
-      <c r="K37" s="22"/>
-      <c r="L37" s="22"/>
-      <c r="M37" s="22"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="17"/>
+      <c r="J37" s="17"/>
+      <c r="K37" s="17"/>
+      <c r="L37" s="17"/>
+      <c r="M37" s="17"/>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="C38" s="20" t="s">
+      <c r="C38" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="D38" s="21"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
-      <c r="I38" s="22"/>
-      <c r="J38" s="22"/>
-      <c r="K38" s="22"/>
-      <c r="L38" s="22"/>
-      <c r="M38" s="22"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="17"/>
+      <c r="J38" s="17"/>
+      <c r="K38" s="17"/>
+      <c r="L38" s="17"/>
+      <c r="M38" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="B12:U12"/>
+    <mergeCell ref="E23:M23"/>
+    <mergeCell ref="E24:M24"/>
+    <mergeCell ref="E25:M25"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="E31:M31"/>
@@ -2139,27 +2185,6 @@
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="B12:U12"/>
-    <mergeCell ref="E23:M23"/>
-    <mergeCell ref="E24:M24"/>
-    <mergeCell ref="E25:M25"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="C14:D14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>